<commit_message>
fixed problems with chromatograms
</commit_message>
<xml_diff>
--- a/tests/data/targets/v0.xlsx
+++ b/tests/data/targets/v0.xlsx
@@ -14,29 +14,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>mz_mean</t>
+  </si>
+  <si>
+    <t>mz_width</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>rt_min</t>
+  </si>
+  <si>
+    <t>rt_max</t>
+  </si>
+  <si>
+    <t>rt_unit</t>
+  </si>
+  <si>
+    <t>intensity_threshold</t>
+  </si>
+  <si>
+    <t>target_filename</t>
+  </si>
   <si>
     <t>peak_label</t>
   </si>
   <si>
-    <t>mz_mean</t>
-  </si>
-  <si>
-    <t>mz_width</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>rt_min</t>
-  </si>
-  <si>
-    <t>rt_max</t>
-  </si>
-  <si>
-    <t>intensity_threshold</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -46,7 +52,10 @@
     <t>3</t>
   </si>
   <si>
-    <t>4</t>
+    <t>s</t>
+  </si>
+  <si>
+    <t>v0.csv</t>
   </si>
 </sst>
 </file>
@@ -404,13 +413,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,97 +444,86 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>151.0605</v>
       </c>
       <c r="C2">
-        <v>151.0605</v>
-      </c>
-      <c r="D2">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>304.2</v>
+      </c>
       <c r="F2">
-        <v>5.07</v>
-      </c>
-      <c r="G2">
-        <v>5.09</v>
+        <v>305.4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>216.0504</v>
       </c>
       <c r="C3">
-        <v>216.0504</v>
-      </c>
-      <c r="D3">
         <v>5</v>
       </c>
+      <c r="E3">
+        <v>238.8</v>
+      </c>
       <c r="F3">
-        <v>3.98</v>
-      </c>
-      <c r="G3">
-        <v>4.39</v>
+        <v>263.4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>115.0032</v>
       </c>
       <c r="C4">
-        <v>115.0032</v>
-      </c>
-      <c r="D4">
         <v>5</v>
       </c>
+      <c r="E4">
+        <v>207</v>
+      </c>
       <c r="F4">
-        <v>3.45</v>
-      </c>
-      <c r="G4">
-        <v>4.39</v>
+        <v>263.4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>273.00061</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1.1</v>
-      </c>
-      <c r="G5">
-        <v>2.22</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="I4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>